<commit_message>
chore: faster unbundled dist executable
</commit_message>
<xml_diff>
--- a/dist/weather_data.xlsx
+++ b/dist/weather_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Python\weather-scraping\dist\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DACADB70-53DC-443E-BDB7-C98DB63F1B67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE92D042-C3F7-494F-8F12-6B04EFBC2F40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17388" yWindow="-10476" windowWidth="17496" windowHeight="30336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-17388" yWindow="-9984" windowWidth="17496" windowHeight="30336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
     <t>description</t>
   </si>
   <si>
-    <t>30.11.2022</t>
+    <t>30.11.2023</t>
   </si>
 </sst>
 </file>
@@ -391,7 +391,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>